<commit_message>
Changed/updated axis and titles to copy into report
</commit_message>
<xml_diff>
--- a/Q4-8withslow.xlsx
+++ b/Q4-8withslow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14246" windowHeight="9669" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="9675" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Q4 - coins with slow" sheetId="4" r:id="rId1"/>
@@ -602,7 +602,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Q4: Min coins vs Amount</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1684,11 +1740,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334150744"/>
-        <c:axId val="334148392"/>
+        <c:axId val="327060432"/>
+        <c:axId val="327060824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334150744"/>
+        <c:axId val="327060432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1801,12 +1857,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334148392"/>
+        <c:crossAx val="327060824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334148392"/>
+        <c:axId val="327060824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1919,7 +1975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334150744"/>
+        <c:crossAx val="327060432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2030,8 +2086,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>V1</a:t>
+              <a:t>Q5</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Min coins vs Amount for V1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3147,11 +3208,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334149960"/>
-        <c:axId val="334151920"/>
+        <c:axId val="327057688"/>
+        <c:axId val="327058080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334149960"/>
+        <c:axId val="327057688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3171,6 +3232,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Amount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3208,12 +3325,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334151920"/>
+        <c:crossAx val="327058080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334151920"/>
+        <c:axId val="327058080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3254,8 +3371,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>min coins</a:t>
+                  <a:t>Min</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Coins</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3326,7 +3448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334149960"/>
+        <c:crossAx val="327057688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3436,9 +3558,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>V2</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Q5 - Min coins vs Amount for V2</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4554,11 +4681,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334146824"/>
-        <c:axId val="334149176"/>
+        <c:axId val="431751736"/>
+        <c:axId val="431757224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334146824"/>
+        <c:axId val="431751736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4578,6 +4705,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Amount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4615,12 +4798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334149176"/>
+        <c:crossAx val="431757224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334149176"/>
+        <c:axId val="431757224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4661,7 +4844,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>min coins</a:t>
+                  <a:t>Min Coins</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4733,7 +4916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334146824"/>
+        <c:crossAx val="431751736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6016,11 +6199,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334153488"/>
-        <c:axId val="334150352"/>
+        <c:axId val="431755264"/>
+        <c:axId val="431755656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334153488"/>
+        <c:axId val="431755264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6133,12 +6316,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334150352"/>
+        <c:crossAx val="431755656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334150352"/>
+        <c:axId val="431755656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6251,7 +6434,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334153488"/>
+        <c:crossAx val="431755264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6362,15 +6545,23 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Q5 - V1</a:t>
+              <a:t>Q5 </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> -</a:t>
+              <a:t>- </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Time vs Amount</a:t>
+              <a:t>Time vs Amount with Slow</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Change </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(Set V1)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7532,11 +7723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334146432"/>
-        <c:axId val="334147608"/>
+        <c:axId val="431756832"/>
+        <c:axId val="431752912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334146432"/>
+        <c:axId val="431756832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7649,12 +7840,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334147608"/>
+        <c:crossAx val="431752912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334147608"/>
+        <c:axId val="431752912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7767,7 +7958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334146432"/>
+        <c:crossAx val="431756832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8672,6 +8863,51 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>time!$K$3:$K$52</c:f>
@@ -9000,11 +9236,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334771896"/>
-        <c:axId val="334769152"/>
+        <c:axId val="431758008"/>
+        <c:axId val="431754088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334771896"/>
+        <c:axId val="431758008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9117,12 +9353,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334769152"/>
+        <c:crossAx val="431754088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334769152"/>
+        <c:axId val="431754088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9235,7 +9471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334771896"/>
+        <c:crossAx val="431758008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12651,7 +12887,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12662,7 +12898,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12673,7 +12909,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12684,7 +12920,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12695,7 +12931,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12706,7 +12942,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12717,7 +12953,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6075189"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12744,7 +12980,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6075189"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12771,7 +13007,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6075189"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12798,7 +13034,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6075189"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12825,7 +13061,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6075189"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12852,7 +13088,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6075189"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -13144,26 +13380,26 @@
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.15234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="12" width="13.921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="14.15234375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="13.921875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -13174,7 +13410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -13203,7 +13439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -13241,7 +13477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -13279,7 +13515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -13317,7 +13553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -13355,7 +13591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -13393,7 +13629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -13431,7 +13667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -13469,7 +13705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -13507,7 +13743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -13545,7 +13781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -13583,7 +13819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -13621,7 +13857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -13659,7 +13895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -13697,7 +13933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -13735,7 +13971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -13773,7 +14009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
@@ -13811,7 +14047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85</v>
       </c>
@@ -13849,7 +14085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
@@ -13887,7 +14123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>95</v>
       </c>
@@ -13925,7 +14161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -13963,7 +14199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105</v>
       </c>
@@ -14001,7 +14237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -14039,7 +14275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>115</v>
       </c>
@@ -14077,7 +14313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>120</v>
       </c>
@@ -14115,7 +14351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>125</v>
       </c>
@@ -14153,7 +14389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>130</v>
       </c>
@@ -14191,7 +14427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>135</v>
       </c>
@@ -14229,7 +14465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>140</v>
       </c>
@@ -14267,7 +14503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>145</v>
       </c>
@@ -14305,7 +14541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>150</v>
       </c>
@@ -14343,7 +14579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>155</v>
       </c>
@@ -14381,7 +14617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>160</v>
       </c>
@@ -14419,7 +14655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>165</v>
       </c>
@@ -14457,7 +14693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>170</v>
       </c>
@@ -14495,7 +14731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>175</v>
       </c>
@@ -14533,7 +14769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>180</v>
       </c>
@@ -14571,7 +14807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>185</v>
       </c>
@@ -14609,7 +14845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>190</v>
       </c>
@@ -14647,7 +14883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>195</v>
       </c>
@@ -14685,7 +14921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>200</v>
       </c>
@@ -14723,7 +14959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>205</v>
       </c>
@@ -14761,7 +14997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>210</v>
       </c>
@@ -14799,7 +15035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>215</v>
       </c>
@@ -14837,7 +15073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>220</v>
       </c>
@@ -14875,7 +15111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>225</v>
       </c>
@@ -14913,7 +15149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>230</v>
       </c>
@@ -14951,7 +15187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>235</v>
       </c>
@@ -14989,7 +15225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>240</v>
       </c>
@@ -15027,7 +15263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>245</v>
       </c>
@@ -15065,7 +15301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>250</v>
       </c>
@@ -15112,24 +15348,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:N52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.15234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15140,7 +15376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -15169,7 +15405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -15208,7 +15444,7 @@
         <v>3.8591524315734203E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -15247,7 +15483,7 @@
         <v>6.4045508438859102E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -15286,7 +15522,7 @@
         <v>9.4836618266036496E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -15325,7 +15561,7 @@
         <v>1.5067116408484701E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -15364,7 +15600,7 @@
         <v>2.5782422628051101E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -15403,7 +15639,7 @@
         <v>2.2621202019301701E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -15442,7 +15678,7 @@
         <v>2.3524407907515799E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -15480,7 +15716,7 @@
         <v>2.73835603390892E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -15518,7 +15754,7 @@
         <v>3.1858534967188399E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -15556,7 +15792,7 @@
         <v>3.9946333148321802E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -15594,7 +15830,7 @@
         <v>7.7634651575930698E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -15632,7 +15868,7 @@
         <v>6.0350575260059697E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -15670,7 +15906,7 @@
         <v>7.0285840030681593E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -15708,7 +15944,7 @@
         <v>8.4490805364012498E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -15746,7 +15982,7 @@
         <v>9.76283455567106E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
@@ -15784,7 +16020,7 @@
         <v>1.30472196038411E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85</v>
       </c>
@@ -15822,7 +16058,7 @@
         <v>2.2793632234270299E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
@@ -15860,7 +16096,7 @@
         <v>1.7243021502864E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>95</v>
       </c>
@@ -15898,7 +16134,7 @@
         <v>3.19365391121007E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -15936,7 +16172,7 @@
         <v>2.0740891579160701E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105</v>
       </c>
@@ -15974,7 +16210,7 @@
         <v>2.2584252687449699E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -16012,7 +16248,7 @@
         <v>5.7304308127861196E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>115</v>
       </c>
@@ -16050,7 +16286,7 @@
         <v>4.09111212562152E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>120</v>
       </c>
@@ -16088,7 +16324,7 @@
         <v>5.4795859047329599E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>125</v>
       </c>
@@ -16126,7 +16362,7 @@
         <v>4.2384989046579898E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>130</v>
       </c>
@@ -16164,7 +16400,7 @@
         <v>3.9297667101294498E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>135</v>
       </c>
@@ -16202,7 +16438,7 @@
         <v>4.4199611785682402E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>140</v>
       </c>
@@ -16240,7 +16476,7 @@
         <v>4.7040604852348599E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>145</v>
       </c>
@@ -16278,7 +16514,7 @@
         <v>5.19877098311472E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>150</v>
       </c>
@@ -16316,7 +16552,7 @@
         <v>5.6598165342513997E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>155</v>
       </c>
@@ -16354,7 +16590,7 @@
         <v>6.1799810162543802E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>160</v>
       </c>
@@ -16392,7 +16628,7 @@
         <v>6.5917607916681203E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>165</v>
       </c>
@@ -16430,7 +16666,7 @@
         <v>7.2560276676600897E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>170</v>
       </c>
@@ -16468,7 +16704,7 @@
         <v>8.1625179409527905E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>175</v>
       </c>
@@ -16506,7 +16742,7 @@
         <v>9.2993257157489805E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>180</v>
       </c>
@@ -16544,7 +16780,7 @@
         <v>1.05724354700447E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>185</v>
       </c>
@@ -16582,7 +16818,7 @@
         <v>1.0271093141875E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>190</v>
       </c>
@@ -16620,7 +16856,7 @@
         <v>1.09698460608731E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>195</v>
       </c>
@@ -16658,7 +16894,7 @@
         <v>1.18611460533184E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>200</v>
       </c>
@@ -16696,7 +16932,7 @@
         <v>1.3157246502951E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>205</v>
       </c>
@@ -16734,7 +16970,7 @@
         <v>1.47752166873038E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>210</v>
       </c>
@@ -16772,7 +17008,7 @@
         <v>1.53869334025245E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>215</v>
       </c>
@@ -16810,7 +17046,7 @@
         <v>1.6497466096935399E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>220</v>
       </c>
@@ -16848,7 +17084,7 @@
         <v>2.3898827802976302E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>225</v>
       </c>
@@ -16886,7 +17122,7 @@
         <v>1.9399220286989401E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>230</v>
       </c>
@@ -16924,7 +17160,7 @@
         <v>2.0429696095851202E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>235</v>
       </c>
@@ -16962,7 +17198,7 @@
         <v>2.1538176049607301E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>240</v>
       </c>
@@ -17000,7 +17236,7 @@
         <v>2.3017791513805898E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>245</v>
       </c>
@@ -17038,7 +17274,7 @@
         <v>2.4593885788794598E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>250</v>
       </c>

</xml_diff>

<commit_message>
Edited stats and added charts for Q8
</commit_message>
<xml_diff>
--- a/Q4-8withslow.xlsx
+++ b/Q4-8withslow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="9675" tabRatio="796" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="9675" tabRatio="796" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Q4 - Min Coins with Slow" sheetId="15" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="Q5 - Time with Slow (V2)" sheetId="21" r:id="rId8"/>
     <sheet name="Q6 - Time with Slow" sheetId="22" r:id="rId9"/>
     <sheet name="time" sheetId="3" r:id="rId10"/>
+    <sheet name="Q8 - Slow" sheetId="24" r:id="rId11"/>
+    <sheet name="Q8 time " sheetId="23" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Q4</t>
   </si>
@@ -97,6 +99,15 @@
   </si>
   <si>
     <t>Slow-V2</t>
+  </si>
+  <si>
+    <t>Number of Denominations</t>
+  </si>
+  <si>
+    <t>Slow-Q4</t>
+  </si>
+  <si>
+    <t>Slow-Q6</t>
   </si>
 </sst>
 </file>
@@ -681,7 +692,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1793,11 +1803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354016552"/>
-        <c:axId val="354008320"/>
+        <c:axId val="322621912"/>
+        <c:axId val="322627400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354016552"/>
+        <c:axId val="322621912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1844,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1901,12 +1910,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354008320"/>
+        <c:crossAx val="322627400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354008320"/>
+        <c:axId val="322627400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1952,7 +1961,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2019,7 +2027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354016552"/>
+        <c:crossAx val="322621912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2033,7 +2041,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2143,7 +2150,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4155,11 +4161,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="422394568"/>
-        <c:axId val="422388688"/>
+        <c:axId val="322622304"/>
+        <c:axId val="322620344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="422394568"/>
+        <c:axId val="322622304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,7 +4202,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4263,12 +4268,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422388688"/>
+        <c:crossAx val="322620344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="422388688"/>
+        <c:axId val="322620344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4314,7 +4319,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4381,7 +4385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422394568"/>
+        <c:crossAx val="322622304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4395,7 +4399,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4502,7 +4505,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6514,11 +6516,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="411470256"/>
-        <c:axId val="411469472"/>
+        <c:axId val="322623088"/>
+        <c:axId val="322624264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="411470256"/>
+        <c:axId val="322623088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6555,7 +6557,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6622,12 +6623,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411469472"/>
+        <c:crossAx val="322624264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="411469472"/>
+        <c:axId val="322624264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6673,7 +6674,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6740,7 +6740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411470256"/>
+        <c:crossAx val="322623088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6754,7 +6754,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6856,7 +6855,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7698,11 +7696,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="411483192"/>
-        <c:axId val="411487896"/>
+        <c:axId val="324125768"/>
+        <c:axId val="324128904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="411483192"/>
+        <c:axId val="324125768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7734,7 +7732,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7801,12 +7798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411487896"/>
+        <c:crossAx val="324128904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="411487896"/>
+        <c:axId val="324128904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7852,7 +7849,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7919,7 +7915,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411483192"/>
+        <c:crossAx val="324125768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7933,7 +7929,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8035,7 +8030,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8833,7 +8827,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -9192,11 +9185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="422371832"/>
-        <c:axId val="422372616"/>
+        <c:axId val="324131256"/>
+        <c:axId val="324128120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="422371832"/>
+        <c:axId val="324131256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9228,7 +9221,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9295,12 +9287,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422372616"/>
+        <c:crossAx val="324128120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="422372616"/>
+        <c:axId val="324128120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9346,7 +9338,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9413,7 +9404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422371832"/>
+        <c:crossAx val="324131256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9427,7 +9418,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9529,7 +9519,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10927,7 +10916,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -11586,11 +11574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="411475352"/>
-        <c:axId val="411468688"/>
+        <c:axId val="324128512"/>
+        <c:axId val="324129296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="411475352"/>
+        <c:axId val="324128512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11622,7 +11610,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11689,12 +11676,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411468688"/>
+        <c:crossAx val="324129296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="411468688"/>
+        <c:axId val="324129296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11740,7 +11727,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11807,7 +11793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411475352"/>
+        <c:crossAx val="324128512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11821,7 +11807,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11923,7 +11908,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13935,11 +13919,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="422375360"/>
-        <c:axId val="422374184"/>
+        <c:axId val="324131648"/>
+        <c:axId val="324129688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="422375360"/>
+        <c:axId val="324131648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13971,7 +13955,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14038,12 +14021,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422374184"/>
+        <c:crossAx val="324129688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="422374184"/>
+        <c:axId val="324129688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14089,7 +14072,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14156,7 +14138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422375360"/>
+        <c:crossAx val="324131648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14170,7 +14152,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15159,11 +15140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="411476136"/>
-        <c:axId val="411476528"/>
+        <c:axId val="324132040"/>
+        <c:axId val="324130472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="411476136"/>
+        <c:axId val="324132040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15262,12 +15243,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411476528"/>
+        <c:crossAx val="324130472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="411476528"/>
+        <c:axId val="324130472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15380,7 +15361,1335 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411476136"/>
+        <c:crossAx val="324132040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time vs Number of Denominations</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for Slow Algorithm (A = 1 to 70)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8 time '!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Slow-Q4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$B$3:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5.7887286473920496E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2809101687845301E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8075186142522399E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2150681017240096E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.03293909764805E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1.31785950057641E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.96857828824419E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.5729051371066398E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>3.6066653310167299E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4.7258195361791399E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>6.3852550817647597E-4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>8.1395272456161595E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>1.0601173839216199E-3</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1.3377710849309099E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8 time '!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Slow-V1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$D$3:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$E$3:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>3.9002072448113203E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.02037304023406E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3342814258265799E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6110861132977401E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5037129973124402E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7230409464281701E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0607972516565307E-5</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>1.20331657202399E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.3869268337541801E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>3.5849062800714601E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>2.5396507384947101E-4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>3.3779900220380898E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>4.1141028209601399E-4</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>5.2197089377976598E-4</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>6.4324681168308401E-4</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>8.0984724325112696E-4</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>9.7172637131315298E-4</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>1.17966899967498E-3</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>1.4169247645916901E-3</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>1.6848074200829801E-3</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>2.1128449014849301E-3</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>2.4045393485749799E-3</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>2.84534487685199E-3</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>3.2310959007592201E-3</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>3.7314719628469099E-3</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>4.3433528973203196E-3</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>5.0212499712614499E-3</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>5.7441020655495797E-3</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>6.5520197325852703E-3</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>7.4854009084606996E-3</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>8.4955135300241093E-3</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>9.6309254411749996E-3</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>1.0886586899901801E-2</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>1.52209077383396E-2</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>1.5327034430208599E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8 time '!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Slow-V2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$G$3:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$H$3:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5.0497420147621597E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1024826695520401E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9911584354303999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2783877619240206E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1536402485035E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.48207875326988E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0034748791886099E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6110861131201E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3541782300971998E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.95768398334439E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8773117964628898E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7353573907903403E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9013140824836206E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.7118313399514594E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.9745821441056196E-5</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1.02472813500753E-4</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>1.20906424581335E-4</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>1.41803324453348E-4</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>1.5079432852189699E-4</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>1.9977272055484699E-4</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>2.0112752938530301E-4</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>2.2645834907280001E-4</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>2.5700313001948401E-4</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>2.8816373315976301E-4</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>3.2240344729075302E-4</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>3.6378669889813799E-4</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>3.8653106535662101E-4</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>4.4396674888389398E-4</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>4.8403624647335098E-4</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>5.3391784439327196E-4</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>6.2042033559919199E-4</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>6.5938135323335696E-4</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>7.0618384016824995E-4</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>7.7515592618055903E-4</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>8.4121312045795096E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8 time '!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Slow-Q6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$J$3:$J$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8 time '!$K$3:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>6.7740441618419002E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5929267483603198E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6703002913249202E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2731754419961106E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.18032587668447E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.2058751079741501E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>3.4535308781460299E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>5.7287886202626805E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>8.2700815512807397E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>1.26067014592522E-3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>1.82689812822895E-3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>2.6439299637732302E-3</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>3.74428106453488E-3</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>5.1817742904907201E-3</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>7.7125571893546501E-3</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>9.8298360106545395E-3</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>1.3266739689494199E-2</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>1.7886432533804501E-2</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>2.3629631393466001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>3.5705042516364402E-2</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>4.2940994380417097E-2</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>5.3145701889506701E-2</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>6.8117037418998799E-2</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>8.7745466727537205E-2</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.111530326369342</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.14394774050730599</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>0.18224724193765501</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>0.224672628920324</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>0.28280640849210598</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>0.34919261604553398</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>0.43506257574613</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>0.53627139366310705</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>0.66468214542600101</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>0.80910686075192595</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>0.99297814898627401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="344780464"/>
+        <c:axId val="344776544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="344780464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Denominations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344776544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="344776544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344780464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15737,6 +17046,46 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -19904,6 +21253,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -19982,6 +21847,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -20182,6 +22058,33 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -27910,4 +29813,858 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.7887286473920496E-6</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.9002072448113203E-6</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5.0497420147621597E-6</v>
+      </c>
+      <c r="J3">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1">
+        <v>6.7740441618419002E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.2809101687845301E-5</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7.02037304023406E-6</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7.1024826695520401E-6</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.5929267483603198E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.8075186142522399E-5</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.3342814258265799E-5</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.9911584354303999E-5</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3.6703002913249202E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.2150681017240096E-5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.6110861132977401E-5</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>9.2783877619240206E-6</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6.2731754419961106E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.03293909764805E-4</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4.5037129973124402E-5</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.1536402485035E-5</v>
+      </c>
+      <c r="J7">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>1.18032587668447E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1.31785950057641E-4</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5.7230409464281701E-5</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.48207875326988E-5</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>2.2058751079741501E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1.96857828824419E-4</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9.0607972516565307E-5</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.0034748791886099E-5</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>3.4535308781460299E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>2.5729051371066398E-4</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>1.20331657202399E-4</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2.6110861131201E-5</v>
+      </c>
+      <c r="J10">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <v>5.7287886202626805E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>3.6066653310167299E-4</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>2.3869268337541801E-4</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3.3541782300971998E-5</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>8.2700815512807397E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>4.7258195361791399E-4</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>3.5849062800714601E-4</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3.95768398334439E-5</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>1.26067014592522E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>6.3852550817647597E-4</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>2.5396507384947101E-4</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4.8773117964628898E-5</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>1.82689812822895E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>8.1395272456161595E-4</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>3.3779900220380898E-4</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5.7353573907903403E-5</v>
+      </c>
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>2.6439299637732302E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>1.0601173839216199E-3</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>4.1141028209601399E-4</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>6.9013140824836206E-5</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>3.74428106453488E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1.3377710849309099E-3</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>5.2197089377976598E-4</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>8.7118313399514594E-5</v>
+      </c>
+      <c r="J16">
+        <v>16</v>
+      </c>
+      <c r="K16">
+        <v>5.1817742904907201E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>6.4324681168308401E-4</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>8.9745821441056196E-5</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>7.7125571893546501E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>8.0984724325112696E-4</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>1.02472813500753E-4</v>
+      </c>
+      <c r="J18">
+        <v>16</v>
+      </c>
+      <c r="K18">
+        <v>9.8298360106545395E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>9.7172637131315298E-4</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>1.20906424581335E-4</v>
+      </c>
+      <c r="J19">
+        <v>16</v>
+      </c>
+      <c r="K19">
+        <v>1.3266739689494199E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>1.17966899967498E-3</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>1.41803324453348E-4</v>
+      </c>
+      <c r="J20">
+        <v>16</v>
+      </c>
+      <c r="K20">
+        <v>1.7886432533804501E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>1.4169247645916901E-3</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>1.5079432852189699E-4</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>2.3629631393466001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>1.6848074200829801E-3</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>1.9977272055484699E-4</v>
+      </c>
+      <c r="J22">
+        <v>16</v>
+      </c>
+      <c r="K22">
+        <v>3.5705042516364402E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>2.1128449014849301E-3</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>2.0112752938530301E-4</v>
+      </c>
+      <c r="J23">
+        <v>16</v>
+      </c>
+      <c r="K23">
+        <v>4.2940994380417097E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>2.4045393485749799E-3</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>2.2645834907280001E-4</v>
+      </c>
+      <c r="J24">
+        <v>16</v>
+      </c>
+      <c r="K24">
+        <v>5.3145701889506701E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>2.84534487685199E-3</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>2.5700313001948401E-4</v>
+      </c>
+      <c r="J25">
+        <v>16</v>
+      </c>
+      <c r="K25">
+        <v>6.8117037418998799E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>3.2310959007592201E-3</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>2.8816373315976301E-4</v>
+      </c>
+      <c r="J26">
+        <v>16</v>
+      </c>
+      <c r="K26">
+        <v>8.7745466727537205E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>3.7314719628469099E-3</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>3.2240344729075302E-4</v>
+      </c>
+      <c r="J27">
+        <v>16</v>
+      </c>
+      <c r="K27">
+        <v>0.111530326369342</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>4.3433528973203196E-3</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>3.6378669889813799E-4</v>
+      </c>
+      <c r="J28">
+        <v>16</v>
+      </c>
+      <c r="K28">
+        <v>0.14394774050730599</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>5.0212499712614499E-3</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>3.8653106535662101E-4</v>
+      </c>
+      <c r="J29">
+        <v>16</v>
+      </c>
+      <c r="K29">
+        <v>0.18224724193765501</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>5.7441020655495797E-3</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>4.4396674888389398E-4</v>
+      </c>
+      <c r="J30">
+        <v>16</v>
+      </c>
+      <c r="K30">
+        <v>0.224672628920324</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>6.5520197325852703E-3</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>4.8403624647335098E-4</v>
+      </c>
+      <c r="J31">
+        <v>16</v>
+      </c>
+      <c r="K31">
+        <v>0.28280640849210598</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>7.4854009084606996E-3</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <v>5.3391784439327196E-4</v>
+      </c>
+      <c r="J32">
+        <v>16</v>
+      </c>
+      <c r="K32">
+        <v>0.34919261604553398</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>8.4955135300241093E-3</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
+        <v>6.2042033559919199E-4</v>
+      </c>
+      <c r="J33">
+        <v>16</v>
+      </c>
+      <c r="K33">
+        <v>0.43506257574613</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>9.6309254411749996E-3</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>6.5938135323335696E-4</v>
+      </c>
+      <c r="J34">
+        <v>16</v>
+      </c>
+      <c r="K34">
+        <v>0.53627139366310705</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>1.0886586899901801E-2</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>7.0618384016824995E-4</v>
+      </c>
+      <c r="J35">
+        <v>16</v>
+      </c>
+      <c r="K35">
+        <v>0.66468214542600101</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>1.52209077383396E-2</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <v>7.7515592618055903E-4</v>
+      </c>
+      <c r="J36">
+        <v>16</v>
+      </c>
+      <c r="K36">
+        <v>0.80910686075192595</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>1.5327034430208599E-2</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <v>8.4121312045795096E-4</v>
+      </c>
+      <c r="J37">
+        <v>16</v>
+      </c>
+      <c r="K37">
+        <v>0.99297814898627401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>